<commit_message>
updated data, added view data page (without data)
</commit_message>
<xml_diff>
--- a/Ping Pong Stats.xlsx
+++ b/Ping Pong Stats.xlsx
@@ -1,21 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10114"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elijahwolf/Documents/GitHub/ping-pong/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3371C56-DD14-D74D-948D-C8424582FEC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="460" yWindow="760" windowWidth="18200" windowHeight="8500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Ping Pong Game Data"/>
-    <sheet r:id="rId2" sheetId="2" name="Player Records"/>
+    <sheet name="Ping Pong Game Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Player Records" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t>Player Name</t>
   </si>
@@ -60,13 +79,27 @@
   </si>
   <si>
     <t>Loser</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>Andrew</t>
+  </si>
+  <si>
+    <t>Eli</t>
+  </si>
+  <si>
+    <t>Lucas</t>
+  </si>
+  <si>
+    <t>Josh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -109,44 +142,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -157,10 +178,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -198,71 +219,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -290,7 +311,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -313,11 +334,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -326,13 +347,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -342,7 +363,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -351,7 +372,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -360,7 +381,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -368,10 +389,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -436,170 +457,251 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="16.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="15.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="4" width="16.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="15.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="4" width="8.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="4" width="8.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
-      <c r="A2" s="7">
+    <row r="2" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
         <v>45316</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>11</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" t="b">
         <f>IF(AND(C2=11,E2=9),TRUE,FALSE)</f>
-      </c>
-      <c r="G2" s="8">
+        <v>0</v>
+      </c>
+      <c r="G2" t="b">
         <f>FALSE</f>
-      </c>
-      <c r="H2" s="8">
+        <v>0</v>
+      </c>
+      <c r="H2" t="str">
         <f>IF(C2&gt;E2,B2,D2)</f>
-      </c>
-      <c r="I2" s="8">
+        <v>Nathan</v>
+      </c>
+      <c r="I2" t="str">
         <f>IF(C2&gt;E2,D2,B2)</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
-      <c r="A3" s="7">
+        <v>Logan</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
         <v>45316</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>11</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>3</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" t="b">
         <f>IF(AND(C3=11,E3=9),TRUE,FALSE)</f>
-      </c>
-      <c r="G3" s="8">
+        <v>0</v>
+      </c>
+      <c r="G3" t="b">
         <f>FALSE</f>
-      </c>
-      <c r="H3" s="8">
+        <v>0</v>
+      </c>
+      <c r="H3" t="str">
         <f>IF(C3&gt;E3,B3,D3)</f>
-      </c>
-      <c r="I3" s="8">
+        <v>Nathan</v>
+      </c>
+      <c r="I3" t="str">
         <f>IF(C3&gt;E3,D3,B3)</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
-      <c r="A4" s="7">
+        <v>Logan</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
         <v>45316</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>11</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>9</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" t="b">
         <f>IF(AND(C4=11,E4=9),TRUE,FALSE)</f>
-      </c>
-      <c r="G4" s="8">
+        <v>1</v>
+      </c>
+      <c r="G4" t="b">
         <f>FALSE</f>
-      </c>
-      <c r="H4" s="8">
+        <v>0</v>
+      </c>
+      <c r="H4" t="str">
         <f>IF(C4&gt;E4,B4,D4)</f>
-      </c>
-      <c r="I4" s="8">
+        <v>Logan</v>
+      </c>
+      <c r="I4" t="str">
         <f>IF(C4&gt;E4,D4,B4)</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
-      <c r="A5" s="7">
+        <v>Ethan</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
         <v>45316</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>7</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>11</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" t="b">
         <f>IF(AND(C5=11,E5=9),TRUE,FALSE)</f>
-      </c>
-      <c r="G5" s="8">
+        <v>0</v>
+      </c>
+      <c r="G5" t="b">
         <f>FALSE</f>
-      </c>
-      <c r="H5" s="8">
+        <v>0</v>
+      </c>
+      <c r="H5" t="str">
         <f>IF(C5&gt;E5, B5, D5)</f>
-      </c>
-      <c r="I5" s="8">
+        <v>Logan</v>
+      </c>
+      <c r="I5" t="str">
         <f>IF(C5&gt;E5,D5,B5)</f>
+        <v>Ethan</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
+        <v>45319</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="1">
+        <v>11</v>
+      </c>
+      <c r="F6" t="b">
+        <f>IF(AND(C6=11,E6=9),TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="G6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H6" t="str">
+        <f>IF(C6&gt;E6, B6, D6)</f>
+        <v>Q</v>
+      </c>
+      <c r="I6" t="str">
+        <f>IF(C6&gt;E6,D6,B6)</f>
+        <v>Nathan</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
+        <v>45319</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="1">
+        <v>12</v>
+      </c>
+      <c r="F7" t="b">
+        <f>IF(AND(C7=11,E7=9),TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="G7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" t="str">
+        <f>IF(C7&gt;E7, B7, D7)</f>
+        <v>Andrew</v>
+      </c>
+      <c r="I7" t="str">
+        <f>IF(C7&gt;E7,D7,B7)</f>
+        <v>Nathan</v>
       </c>
     </row>
   </sheetData>
@@ -608,63 +710,135 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" style="4" width="15.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.5" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <f>COUNTIF('Ping Pong Game Data'!$H$2:$H$10000, A2)</f>
-      </c>
-      <c r="C2" s="3">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2">
         <f>COUNTIF('Ping Pong Game Data'!$I$2:$I$10000, A2)</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
-      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <f>COUNTIF('Ping Pong Game Data'!$H$2:$H$10000, A3)</f>
-      </c>
-      <c r="C3" s="3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2">
         <f>COUNTIF('Ping Pong Game Data'!$I$2:$I$10000, A3)</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
-      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <f>COUNTIF('Ping Pong Game Data'!$H$2:$H$10000, A4)</f>
-      </c>
-      <c r="C4" s="3">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2">
         <f>COUNTIF('Ping Pong Game Data'!$I$2:$I$10000, A4)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="2">
+        <f>COUNTIF('Ping Pong Game Data'!$H$2:$H$10000, A5)</f>
+        <v>1</v>
+      </c>
+      <c r="C5" s="2">
+        <f>COUNTIF('Ping Pong Game Data'!$I$2:$I$10000, A5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="2">
+        <f>COUNTIF('Ping Pong Game Data'!$H$2:$H$10000, A6)</f>
+        <v>1</v>
+      </c>
+      <c r="C6" s="2">
+        <f>COUNTIF('Ping Pong Game Data'!$I$2:$I$10000, A6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="2">
+        <f>COUNTIF('Ping Pong Game Data'!$H$2:$H$10000, A7)</f>
+        <v>0</v>
+      </c>
+      <c r="C7" s="2">
+        <f>COUNTIF('Ping Pong Game Data'!$I$2:$I$10000, A7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="2">
+        <f>COUNTIF('Ping Pong Game Data'!$H$2:$H$10000, A8)</f>
+        <v>0</v>
+      </c>
+      <c r="C8" s="2">
+        <f>COUNTIF('Ping Pong Game Data'!$I$2:$I$10000, A8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="2">
+        <f>COUNTIF('Ping Pong Game Data'!$H$2:$H$10000, A9)</f>
+        <v>0</v>
+      </c>
+      <c r="C9" s="2">
+        <f>COUNTIF('Ping Pong Game Data'!$I$2:$I$10000, A9)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated data, refined add_data() function, added empty text file
</commit_message>
<xml_diff>
--- a/Ping Pong Stats.xlsx
+++ b/Ping Pong Stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elijahwolf/Documents/GitHub/ping-pong/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3371C56-DD14-D74D-948D-C8424582FEC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CADFE1CF-E798-6F43-9348-87373C749195}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="460" yWindow="760" windowWidth="18200" windowHeight="8500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="460" yWindow="760" windowWidth="24240" windowHeight="13540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ping Pong Game Data" sheetId="1" r:id="rId1"/>
@@ -33,8 +33,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="22">
   <si>
     <t>Player Name</t>
   </si>
@@ -94,12 +116,21 @@
   </si>
   <si>
     <t>Josh</t>
+  </si>
+  <si>
+    <t>Eric</t>
+  </si>
+  <si>
+    <t>Win %</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -142,7 +173,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -156,6 +187,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,10 +493,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -524,7 +556,7 @@
         <v>11</v>
       </c>
       <c r="F2" t="b">
-        <f>IF(AND(C2=11,E2=9),TRUE,FALSE)</f>
+        <f t="shared" ref="F2:F12" si="0">IF(AND(C2=11,E2=9),TRUE,FALSE)</f>
         <v>0</v>
       </c>
       <c r="G2" t="b">
@@ -536,7 +568,7 @@
         <v>Nathan</v>
       </c>
       <c r="I2" t="str">
-        <f>IF(C2&gt;E2,D2,B2)</f>
+        <f t="shared" ref="I2:I12" si="1">IF(C2&gt;E2,D2,B2)</f>
         <v>Logan</v>
       </c>
     </row>
@@ -557,7 +589,7 @@
         <v>3</v>
       </c>
       <c r="F3" t="b">
-        <f>IF(AND(C3=11,E3=9),TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G3" t="b">
@@ -569,7 +601,7 @@
         <v>Nathan</v>
       </c>
       <c r="I3" t="str">
-        <f>IF(C3&gt;E3,D3,B3)</f>
+        <f t="shared" si="1"/>
         <v>Logan</v>
       </c>
     </row>
@@ -590,7 +622,7 @@
         <v>9</v>
       </c>
       <c r="F4" t="b">
-        <f>IF(AND(C4=11,E4=9),TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G4" t="b">
@@ -602,7 +634,7 @@
         <v>Logan</v>
       </c>
       <c r="I4" t="str">
-        <f>IF(C4&gt;E4,D4,B4)</f>
+        <f t="shared" si="1"/>
         <v>Ethan</v>
       </c>
     </row>
@@ -623,7 +655,7 @@
         <v>11</v>
       </c>
       <c r="F5" t="b">
-        <f>IF(AND(C5=11,E5=9),TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G5" t="b">
@@ -635,7 +667,7 @@
         <v>Logan</v>
       </c>
       <c r="I5" t="str">
-        <f>IF(C5&gt;E5,D5,B5)</f>
+        <f t="shared" si="1"/>
         <v>Ethan</v>
       </c>
     </row>
@@ -656,7 +688,7 @@
         <v>11</v>
       </c>
       <c r="F6" t="b">
-        <f>IF(AND(C6=11,E6=9),TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G6" t="b">
@@ -668,7 +700,7 @@
         <v>Q</v>
       </c>
       <c r="I6" t="str">
-        <f>IF(C6&gt;E6,D6,B6)</f>
+        <f t="shared" si="1"/>
         <v>Nathan</v>
       </c>
     </row>
@@ -689,7 +721,7 @@
         <v>12</v>
       </c>
       <c r="F7" t="b">
-        <f>IF(AND(C7=11,E7=9),TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G7" t="b">
@@ -700,8 +732,272 @@
         <v>Andrew</v>
       </c>
       <c r="I7" t="str">
-        <f>IF(C7&gt;E7,D7,B7)</f>
+        <f t="shared" si="1"/>
         <v>Nathan</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
+        <v>45319</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="1">
+        <v>3</v>
+      </c>
+      <c r="F8" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G8" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H8" t="str">
+        <f>IF(C8&gt;E8, B8, D8)</f>
+        <v>Ethan</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="1"/>
+        <v>Eric</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="4">
+        <v>45319</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="1">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="1">
+        <v>7</v>
+      </c>
+      <c r="F9" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G9" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="H9" t="str">
+        <f>IF(C9&gt;E9, B9, D9)</f>
+        <v>Andrew</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" si="1"/>
+        <v>Nathan</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="4">
+        <v>45319</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="1">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="1">
+        <v>11</v>
+      </c>
+      <c r="F10" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G10" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H10" t="str">
+        <f>IF(C10&gt;E10, B10, D10)</f>
+        <v>Andrew</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="1"/>
+        <v>Nathan</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="4">
+        <v>45319</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="1">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="1">
+        <v>11</v>
+      </c>
+      <c r="F11" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G11" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H11" t="str">
+        <f>IF(C11&gt;E11, B11, D11)</f>
+        <v>Nathan</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="1"/>
+        <v>Andrew</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="4">
+        <v>45319</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="1">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="1">
+        <v>11</v>
+      </c>
+      <c r="F12" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G12" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H12" t="str">
+        <f>IF(C12&gt;E12, B12, D12)</f>
+        <v>Logan</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="1"/>
+        <v>Nathan</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="4">
+        <v>45319</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="1">
+        <v>11</v>
+      </c>
+      <c r="D13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="1">
+        <v>5</v>
+      </c>
+      <c r="F13" t="b">
+        <f t="shared" ref="F13:F15" si="2">IF(AND(C13=11,E13=9),TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="G13" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H13" t="str">
+        <f>IF(C13&gt;E13, B13, D13)</f>
+        <v>Andrew</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" ref="I13:I15" si="3">IF(C13&gt;E13,D13,B13)</f>
+        <v>Logan</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="4">
+        <v>45319</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="1">
+        <v>11</v>
+      </c>
+      <c r="D14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" s="1">
+        <v>3</v>
+      </c>
+      <c r="F14" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G14" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H14" t="str">
+        <f>IF(C14&gt;E14, B14, D14)</f>
+        <v>Andrew</v>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" si="3"/>
+        <v>Nathan</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="4">
+        <v>45319</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="1">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="1">
+        <v>11</v>
+      </c>
+      <c r="F15" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G15" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H15" t="str">
+        <f>IF(C15&gt;E15, B15, D15)</f>
+        <v>Nathan</v>
+      </c>
+      <c r="I15" t="str">
+        <f t="shared" si="3"/>
+        <v>Logan</v>
       </c>
     </row>
   </sheetData>
@@ -714,10 +1010,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -726,7 +1022,7 @@
     <col min="2" max="3" width="12.5" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -736,62 +1032,81 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B2" s="2">
         <f>COUNTIF('Ping Pong Game Data'!$H$2:$H$10000, A2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" s="2">
         <f>COUNTIF('Ping Pong Game Data'!$I$2:$I$10000, A2)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="5">
+        <f>IF((B2+C2)&gt;0, B2/(B2+C2), 0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B3" s="2">
         <f>COUNTIF('Ping Pong Game Data'!$H$2:$H$10000, A3)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C3" s="2">
         <f>COUNTIF('Ping Pong Game Data'!$I$2:$I$10000, A3)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5">
+        <f>IF((B3+C3)&gt;0, B3/(B3+C3), 0)</f>
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2">
         <f>COUNTIF('Ping Pong Game Data'!$H$2:$H$10000, A4)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C4" s="2">
         <f>COUNTIF('Ping Pong Game Data'!$I$2:$I$10000, A4)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="D4" s="5">
+        <f>IF((B4+C4)&gt;0, B4/(B4+C4), 0)</f>
+        <v>0.42857142857142855</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2">
         <f>COUNTIF('Ping Pong Game Data'!$H$2:$H$10000, A5)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C5" s="2">
         <f>COUNTIF('Ping Pong Game Data'!$I$2:$I$10000, A5)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="D5" s="5">
+        <f>IF((B5+C5)&gt;0, B5/(B5+C5), 0)</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2">
         <f>COUNTIF('Ping Pong Game Data'!$H$2:$H$10000, A6)</f>
@@ -799,10 +1114,14 @@
       </c>
       <c r="C6" s="2">
         <f>COUNTIF('Ping Pong Game Data'!$I$2:$I$10000, A6)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="D6" s="5">
+        <f>IF((B6+C6)&gt;0, B6/(B6+C6), 0)</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -814,8 +1133,12 @@
         <f>COUNTIF('Ping Pong Game Data'!$I$2:$I$10000, A7)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7" s="5">
+        <f>IF((B7+C7)&gt;0, B7/(B7+C7), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -827,8 +1150,12 @@
         <f>COUNTIF('Ping Pong Game Data'!$I$2:$I$10000, A8)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8" s="5">
+        <f>IF((B8+C8)&gt;0, B8/(B8+C8), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -840,8 +1167,159 @@
         <f>COUNTIF('Ping Pong Game Data'!$I$2:$I$10000, A9)</f>
         <v>0</v>
       </c>
+      <c r="D9" s="5">
+        <f>IF((B9+C9)&gt;0, B9/(B9+C9), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="2">
+        <f>COUNTIF('Ping Pong Game Data'!$H$2:$H$10000, A10)</f>
+        <v>0</v>
+      </c>
+      <c r="C10" s="2">
+        <f>COUNTIF('Ping Pong Game Data'!$I$2:$I$10000, A10)</f>
+        <v>1</v>
+      </c>
+      <c r="D10" s="5">
+        <f>IF((B10+C10)&gt;0, B10/(B10+C10), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="str" cm="1">
+        <f t="array" ref="A11:D19">_xlfn._xlws.SORT(A2:D10,4,-1)</f>
+        <v>Q</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="str">
+        <v>Andrew</v>
+      </c>
+      <c r="B12" s="1">
+        <v>5</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
+      <c r="D12" s="5">
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="str">
+        <v>Logan</v>
+      </c>
+      <c r="B13" s="1">
+        <v>3</v>
+      </c>
+      <c r="C13" s="1">
+        <v>4</v>
+      </c>
+      <c r="D13" s="5">
+        <v>0.42857142857142855</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="str">
+        <v>Nathan</v>
+      </c>
+      <c r="B14" s="1">
+        <v>4</v>
+      </c>
+      <c r="C14" s="1">
+        <v>6</v>
+      </c>
+      <c r="D14" s="5">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="str">
+        <v>Ethan</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1">
+        <v>2</v>
+      </c>
+      <c r="D15" s="5">
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="str">
+        <v>Eli</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0</v>
+      </c>
+      <c r="D16" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="str">
+        <v>Lucas</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0</v>
+      </c>
+      <c r="D17" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="str">
+        <v>Josh</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0</v>
+      </c>
+      <c r="D18" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="str">
+        <v>Eric</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1</v>
+      </c>
+      <c r="D19" s="5">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D10">
+    <sortCondition descending="1" ref="D2:D10"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added additional data to spreadsheet
</commit_message>
<xml_diff>
--- a/Ping Pong Stats.xlsx
+++ b/Ping Pong Stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elijahwolf/Documents/GitHub/ping-pong/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E81E11-BED4-8145-AB90-765A32BEFA1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3D50FF3-1ACB-A845-A2CC-19C8F31D4BF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="11720" windowHeight="13060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="22120" windowHeight="17080" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ping Pong Game Data" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="20">
   <si>
     <t>Player Name</t>
   </si>
@@ -109,19 +109,13 @@
     <t>Andrew</t>
   </si>
   <si>
-    <t>Eli</t>
-  </si>
-  <si>
-    <t>Lucas</t>
-  </si>
-  <si>
-    <t>Josh</t>
-  </si>
-  <si>
     <t>Eric</t>
   </si>
   <si>
     <t>Win %</t>
+  </si>
+  <si>
+    <t>Score Diff.</t>
   </si>
 </sst>
 </file>
@@ -173,7 +167,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -188,6 +182,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -493,10 +488,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -663,7 +658,7 @@
         <v>0</v>
       </c>
       <c r="H5" t="str">
-        <f t="shared" ref="H5:H21" si="2">IF(C5&gt;E5, B5, D5)</f>
+        <f t="shared" ref="H5:H26" si="2">IF(C5&gt;E5, B5, D5)</f>
         <v>Logan</v>
       </c>
       <c r="I5" t="str">
@@ -747,7 +742,7 @@
         <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E8" s="1">
         <v>3</v>
@@ -918,7 +913,7 @@
         <v>5</v>
       </c>
       <c r="F13" t="b">
-        <f t="shared" ref="F13:F21" si="3">IF(AND(C13=11,E13=9),TRUE,FALSE)</f>
+        <f t="shared" ref="F13:F26" si="3">IF(AND(C13=11,E13=9),TRUE,FALSE)</f>
         <v>0</v>
       </c>
       <c r="G13" t="b">
@@ -930,7 +925,7 @@
         <v>Andrew</v>
       </c>
       <c r="I13" t="str">
-        <f t="shared" ref="I13:I21" si="4">IF(C13&gt;E13,D13,B13)</f>
+        <f t="shared" ref="I13:I26" si="4">IF(C13&gt;E13,D13,B13)</f>
         <v>Logan</v>
       </c>
     </row>
@@ -1167,7 +1162,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
-        <v>45319</v>
+        <v>45320</v>
       </c>
       <c r="B21" t="s">
         <v>4</v>
@@ -1194,6 +1189,171 @@
         <v>Andrew</v>
       </c>
       <c r="I21" t="str">
+        <f t="shared" si="4"/>
+        <v>Nathan</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="4">
+        <v>45320</v>
+      </c>
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="1">
+        <v>7</v>
+      </c>
+      <c r="D22" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="1">
+        <v>11</v>
+      </c>
+      <c r="F22" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G22" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H22" t="str">
+        <f t="shared" si="2"/>
+        <v>Andrew</v>
+      </c>
+      <c r="I22" t="str">
+        <f t="shared" si="4"/>
+        <v>Ethan</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="4">
+        <v>45320</v>
+      </c>
+      <c r="B23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="1">
+        <v>11</v>
+      </c>
+      <c r="D23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" s="1">
+        <v>6</v>
+      </c>
+      <c r="F23" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G23" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="H23" t="str">
+        <f t="shared" si="2"/>
+        <v>Nathan</v>
+      </c>
+      <c r="I23" t="str">
+        <f t="shared" si="4"/>
+        <v>Ethan</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="4">
+        <v>45320</v>
+      </c>
+      <c r="B24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="1">
+        <v>11</v>
+      </c>
+      <c r="D24" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="1">
+        <v>8</v>
+      </c>
+      <c r="F24" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G24" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H24" t="str">
+        <f t="shared" si="2"/>
+        <v>Nathan</v>
+      </c>
+      <c r="I24" t="str">
+        <f t="shared" si="4"/>
+        <v>Andrew</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="4">
+        <v>45320</v>
+      </c>
+      <c r="B25" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="1">
+        <v>11</v>
+      </c>
+      <c r="D25" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="1">
+        <v>9</v>
+      </c>
+      <c r="F25" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G25" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H25" t="str">
+        <f t="shared" si="2"/>
+        <v>Nathan</v>
+      </c>
+      <c r="I25" t="str">
+        <f t="shared" si="4"/>
+        <v>Andrew</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="4">
+        <v>45320</v>
+      </c>
+      <c r="B26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="1">
+        <v>4</v>
+      </c>
+      <c r="D26" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26" s="1">
+        <v>11</v>
+      </c>
+      <c r="F26" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G26" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H26" t="str">
+        <f t="shared" si="2"/>
+        <v>Ethan</v>
+      </c>
+      <c r="I26" t="str">
         <f t="shared" si="4"/>
         <v>Nathan</v>
       </c>
@@ -1208,19 +1368,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="7.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1231,10 +1392,13 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1247,28 +1411,37 @@
         <v>0</v>
       </c>
       <c r="D2" s="5">
-        <f t="shared" ref="D2:D10" si="0">IF((B2+C2)&gt;0, B2/(B2+C2), 0)</f>
+        <f t="shared" ref="D2:D6" si="0">IF((B2+C2)&gt;0, B2/(B2+C2), 0)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E2" s="6">
+        <f>SUMIFS('Ping Pong Game Data'!$C$2:$C$10000,'Ping Pong Game Data'!$B$2:$B$10000,$A2)+SUMIFS('Ping Pong Game Data'!$E$2:$E$10000,'Ping Pong Game Data'!$D$2:$D$10000,$A2)-SUMIFS('Ping Pong Game Data'!$C$2:$C$10000,'Ping Pong Game Data'!$D$2:$D$10000,$A2)-SUMIFS('Ping Pong Game Data'!$E$2:$E$10000,'Ping Pong Game Data'!$B$2:$B$10000,$A2)</f>
+        <v>7</v>
+      </c>
+      <c r="F2" s="6"/>
+    </row>
+    <row r="3" spans="1:6" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="2">
         <f>COUNTIF('Ping Pong Game Data'!$H$2:$H$10000, A3)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" s="2">
         <f>COUNTIF('Ping Pong Game Data'!$I$2:$I$10000, A3)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D3" s="5">
         <f t="shared" si="0"/>
-        <v>0.875</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0.72727272727272729</v>
+      </c>
+      <c r="E3" s="6">
+        <f>SUMIFS('Ping Pong Game Data'!$C$2:$C$10000,'Ping Pong Game Data'!$B$2:$B$10000,$A3)+SUMIFS('Ping Pong Game Data'!$E$2:$E$10000,'Ping Pong Game Data'!$D$2:$D$10000,$A3)-SUMIFS('Ping Pong Game Data'!$C$2:$C$10000,'Ping Pong Game Data'!$D$2:$D$10000,$A3)-SUMIFS('Ping Pong Game Data'!$E$2:$E$10000,'Ping Pong Game Data'!$B$2:$B$10000,$A3)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1284,42 +1457,54 @@
         <f t="shared" si="0"/>
         <v>0.44444444444444442</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="E4" s="6">
+        <f>SUMIFS('Ping Pong Game Data'!$C$2:$C$10000,'Ping Pong Game Data'!$B$2:$B$10000,$A4)+SUMIFS('Ping Pong Game Data'!$E$2:$E$10000,'Ping Pong Game Data'!$D$2:$D$10000,$A4)-SUMIFS('Ping Pong Game Data'!$C$2:$C$10000,'Ping Pong Game Data'!$D$2:$D$10000,$A4)-SUMIFS('Ping Pong Game Data'!$E$2:$E$10000,'Ping Pong Game Data'!$B$2:$B$10000,$A4)</f>
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2">
         <f>COUNTIF('Ping Pong Game Data'!$H$2:$H$10000, A5)</f>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C5" s="2">
         <f>COUNTIF('Ping Pong Game Data'!$I$2:$I$10000, A5)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D5" s="5">
         <f t="shared" si="0"/>
-        <v>0.4375</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+        <v>0.5</v>
+      </c>
+      <c r="E5" s="6">
+        <f>SUMIFS('Ping Pong Game Data'!$C$2:$C$10000,'Ping Pong Game Data'!$B$2:$B$10000,$A5)+SUMIFS('Ping Pong Game Data'!$E$2:$E$10000,'Ping Pong Game Data'!$D$2:$D$10000,$A5)-SUMIFS('Ping Pong Game Data'!$C$2:$C$10000,'Ping Pong Game Data'!$D$2:$D$10000,$A5)-SUMIFS('Ping Pong Game Data'!$E$2:$E$10000,'Ping Pong Game Data'!$B$2:$B$10000,$A5)</f>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="2">
         <f>COUNTIF('Ping Pong Game Data'!$H$2:$H$10000, A6)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" s="2">
         <f>COUNTIF('Ping Pong Game Data'!$I$2:$I$10000, A6)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D6" s="5">
         <f t="shared" si="0"/>
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+        <v>0.25</v>
+      </c>
+      <c r="E6" s="6">
+        <f>SUMIFS('Ping Pong Game Data'!$C$2:$C$10000,'Ping Pong Game Data'!$B$2:$B$10000,$A6)+SUMIFS('Ping Pong Game Data'!$E$2:$E$10000,'Ping Pong Game Data'!$D$2:$D$10000,$A6)-SUMIFS('Ping Pong Game Data'!$C$2:$C$10000,'Ping Pong Game Data'!$D$2:$D$10000,$A6)-SUMIFS('Ping Pong Game Data'!$E$2:$E$10000,'Ping Pong Game Data'!$B$2:$B$10000,$A6)</f>
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1329,190 +1514,165 @@
       </c>
       <c r="C7" s="2">
         <f>COUNTIF('Ping Pong Game Data'!$I$2:$I$10000, A7)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="2">
-        <f>COUNTIF('Ping Pong Game Data'!$H$2:$H$10000, A8)</f>
-        <v>0</v>
-      </c>
-      <c r="C8" s="2">
-        <f>COUNTIF('Ping Pong Game Data'!$I$2:$I$10000, A8)</f>
-        <v>0</v>
-      </c>
-      <c r="D8" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="2">
-        <f>COUNTIF('Ping Pong Game Data'!$H$2:$H$10000, A9)</f>
-        <v>0</v>
-      </c>
-      <c r="C9" s="2">
-        <f>COUNTIF('Ping Pong Game Data'!$I$2:$I$10000, A9)</f>
-        <v>0</v>
-      </c>
-      <c r="D9" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="2">
-        <f>COUNTIF('Ping Pong Game Data'!$H$2:$H$10000, A10)</f>
-        <v>0</v>
-      </c>
-      <c r="C10" s="2">
-        <f>COUNTIF('Ping Pong Game Data'!$I$2:$I$10000, A10)</f>
+        <f>IF((B7+C7)&gt;0, B7/(B7+C7), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="6">
+        <f>SUMIFS('Ping Pong Game Data'!$C$2:$C$10000,'Ping Pong Game Data'!$B$2:$B$10000,$A7)+SUMIFS('Ping Pong Game Data'!$E$2:$E$10000,'Ping Pong Game Data'!$D$2:$D$10000,$A7)-SUMIFS('Ping Pong Game Data'!$C$2:$C$10000,'Ping Pong Game Data'!$D$2:$D$10000,$A7)-SUMIFS('Ping Pong Game Data'!$E$2:$E$10000,'Ping Pong Game Data'!$B$2:$B$10000,$A7)</f>
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="6"/>
+    </row>
+    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="D12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="D13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="D14" s="5"/>
+    </row>
+    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="D15" s="5"/>
+    </row>
+    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="D16" s="5"/>
+    </row>
+    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="D17" s="5"/>
+    </row>
+    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="D18" s="5"/>
+    </row>
+    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="D19" s="5"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="str" cm="1">
+        <f t="array" ref="A20:E25">_xlfn._xlws.SORT(A2:E7,4,-1)</f>
+        <v>Q</v>
+      </c>
+      <c r="B20" s="1">
         <v>1</v>
       </c>
-      <c r="D10" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="str" cm="1">
-        <f t="array" ref="A11:D19">_xlfn._xlws.SORT(A2:D10,4,-1)</f>
-        <v>Q</v>
-      </c>
-      <c r="B11" s="1">
+      <c r="C20" s="1">
+        <v>0</v>
+      </c>
+      <c r="D20" s="5">
         <v>1</v>
       </c>
-      <c r="C11" s="1">
-        <v>0</v>
-      </c>
-      <c r="D11" s="5">
+      <c r="E20">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="str">
+        <v>Andrew</v>
+      </c>
+      <c r="B21" s="1">
+        <v>8</v>
+      </c>
+      <c r="C21" s="1">
+        <v>3</v>
+      </c>
+      <c r="D21" s="5">
+        <v>0.72727272727272729</v>
+      </c>
+      <c r="E21">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="str">
+        <v>Nathan</v>
+      </c>
+      <c r="B22" s="1">
+        <v>10</v>
+      </c>
+      <c r="C22" s="1">
+        <v>10</v>
+      </c>
+      <c r="D22" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="E22">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="str">
+        <v>Logan</v>
+      </c>
+      <c r="B23" s="1">
+        <v>4</v>
+      </c>
+      <c r="C23" s="1">
+        <v>5</v>
+      </c>
+      <c r="D23" s="5">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="E23">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="str">
+        <v>Ethan</v>
+      </c>
+      <c r="B24" s="1">
+        <v>2</v>
+      </c>
+      <c r="C24" s="1">
+        <v>6</v>
+      </c>
+      <c r="D24" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="E24">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="str">
+        <v>Eric</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0</v>
+      </c>
+      <c r="C25" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="str">
-        <v>Andrew</v>
-      </c>
-      <c r="B12" s="1">
-        <v>7</v>
-      </c>
-      <c r="C12" s="1">
-        <v>1</v>
-      </c>
-      <c r="D12" s="5">
-        <v>0.875</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="str">
-        <v>Logan</v>
-      </c>
-      <c r="B13" s="1">
-        <v>4</v>
-      </c>
-      <c r="C13" s="1">
-        <v>5</v>
-      </c>
-      <c r="D13" s="5">
-        <v>0.44444444444444442</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="str">
-        <v>Nathan</v>
-      </c>
-      <c r="B14" s="1">
-        <v>7</v>
-      </c>
-      <c r="C14" s="1">
-        <v>9</v>
-      </c>
-      <c r="D14" s="5">
-        <v>0.4375</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="str">
-        <v>Ethan</v>
-      </c>
-      <c r="B15" s="1">
-        <v>1</v>
-      </c>
-      <c r="C15" s="1">
-        <v>4</v>
-      </c>
-      <c r="D15" s="5">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="str">
-        <v>Eli</v>
-      </c>
-      <c r="B16" s="1">
-        <v>0</v>
-      </c>
-      <c r="C16" s="1">
-        <v>0</v>
-      </c>
-      <c r="D16" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="str">
-        <v>Lucas</v>
-      </c>
-      <c r="B17" s="1">
-        <v>0</v>
-      </c>
-      <c r="C17" s="1">
-        <v>0</v>
-      </c>
-      <c r="D17" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="str">
-        <v>Josh</v>
-      </c>
-      <c r="B18" s="1">
-        <v>0</v>
-      </c>
-      <c r="C18" s="1">
-        <v>0</v>
-      </c>
-      <c r="D18" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="str">
-        <v>Eric</v>
-      </c>
-      <c r="B19" s="1">
-        <v>0</v>
-      </c>
-      <c r="C19" s="1">
-        <v>1</v>
-      </c>
-      <c r="D19" s="5">
-        <v>0</v>
-      </c>
+      <c r="D25" s="5">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D26" s="5"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D27" s="5"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D10">

</xml_diff>